<commit_message>
Added Basic File Reading
</commit_message>
<xml_diff>
--- a/Jetpack/Assets/Resources/fish_patterns.xlsx
+++ b/Jetpack/Assets/Resources/fish_patterns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding Projects\School\ecs189L\back-to-the-jungle\Jetpack\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A68F23B-C3DB-41A4-91D8-E71BD686B8EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{334172E0-E393-43A1-8B9C-45C9F0B04F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D6B53B84-B4B8-429A-BFC6-3A192A739905}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
   <si>
     <t>D6</t>
   </si>
@@ -68,9 +68,6 @@
   </si>
   <si>
     <t>I2</t>
-  </si>
-  <si>
-    <t>BRUH</t>
   </si>
 </sst>
 </file>
@@ -447,23 +444,20 @@
   <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.28515625" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:18" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="H2" s="1"/>

</xml_diff>

<commit_message>
Added Working Pattern Reading
</commit_message>
<xml_diff>
--- a/Jetpack/Assets/Resources/fish_patterns.xlsx
+++ b/Jetpack/Assets/Resources/fish_patterns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding Projects\School\ecs189L\back-to-the-jungle\Jetpack\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{334172E0-E393-43A1-8B9C-45C9F0B04F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8FA1AB-76FE-413E-AB4A-8504A3CF73EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D6B53B84-B4B8-429A-BFC6-3A192A739905}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{D6B53B84-B4B8-429A-BFC6-3A192A739905}"/>
   </bookViews>
   <sheets>
     <sheet name="BEAN" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="7">
   <si>
     <t>D6</t>
   </si>
@@ -56,9 +56,6 @@
   </si>
   <si>
     <t>H2</t>
-  </si>
-  <si>
-    <t>D2</t>
   </si>
   <si>
     <t>F4</t>
@@ -443,7 +440,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BEEA55C-653B-49A5-9FC5-07B0418692D5}">
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -586,17 +583,17 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.28515625" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -634,7 +631,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -672,7 +669,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -688,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B783E41-6E03-40D6-9F79-8BFA25D1C465}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.28515625" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -738,7 +735,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T6" sqref="T6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.28515625" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -748,7 +745,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -789,7 +786,7 @@
   <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.28515625" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>